<commit_message>
format converting logic building initiated
</commit_message>
<xml_diff>
--- a/miscellenious_discounts/output_files/output_extra_discounts.xlsx
+++ b/miscellenious_discounts/output_files/output_extra_discounts.xlsx
@@ -1718,7 +1718,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I85"/>
+  <dimension ref="A1:J85"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1729,45 +1729,50 @@
     <row r="1">
       <c r="A1" s="6" t="inlineStr">
         <is>
+          <t>SHAPE</t>
+        </is>
+      </c>
+      <c r="B1" s="6" t="inlineStr">
+        <is>
           <t>CUT</t>
         </is>
       </c>
-      <c r="B1" s="6" t="inlineStr">
+      <c r="C1" s="6" t="inlineStr">
         <is>
           <t>POLY</t>
         </is>
       </c>
-      <c r="C1" s="6" t="inlineStr">
+      <c r="D1" s="6" t="inlineStr">
         <is>
           <t>SYM</t>
         </is>
       </c>
-      <c r="D1" s="6" t="inlineStr">
+      <c r="E1" s="6" t="inlineStr">
         <is>
           <t>FLUO</t>
         </is>
       </c>
-      <c r="E1" s="6" t="inlineStr">
+      <c r="F1" s="6" t="inlineStr">
         <is>
           <t>SIZE</t>
         </is>
       </c>
-      <c r="F1" s="6" t="inlineStr">
+      <c r="G1" s="6" t="inlineStr">
         <is>
           <t>DIAMETER_MIN</t>
         </is>
       </c>
-      <c r="G1" s="6" t="inlineStr">
+      <c r="H1" s="6" t="inlineStr">
         <is>
           <t>DIAMETER_MAX</t>
         </is>
       </c>
-      <c r="H1" s="6" t="inlineStr">
+      <c r="I1" s="6" t="inlineStr">
         <is>
           <t>KEY_COLOR_CLARITY</t>
         </is>
       </c>
-      <c r="I1" s="6" t="inlineStr">
+      <c r="J1" s="6" t="inlineStr">
         <is>
           <t>DISCOUNT</t>
         </is>
@@ -1776,7 +1781,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>EX</t>
+          <t>RO</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -1791,31 +1796,36 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
+          <t>EX</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
           <t>NONE</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="F2" t="inlineStr">
         <is>
           <t>0.35-0.399</t>
         </is>
       </c>
-      <c r="F2" t="n">
+      <c r="G2" t="n">
         <v>4.5</v>
       </c>
-      <c r="G2" t="n">
-        <v>100000</v>
-      </c>
       <c r="H2" t="n">
-        <v>1</v>
+        <v>100000</v>
       </c>
       <c r="I2" t="n">
+        <v>1</v>
+      </c>
+      <c r="J2" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>EX</t>
+          <t>RO</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -1830,31 +1840,36 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
+          <t>EX</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
           <t>FAINT</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="F3" t="inlineStr">
         <is>
           <t>0.35-0.399</t>
         </is>
       </c>
-      <c r="F3" t="n">
+      <c r="G3" t="n">
         <v>4.5</v>
       </c>
-      <c r="G3" t="n">
-        <v>100000</v>
-      </c>
       <c r="H3" t="n">
-        <v>1</v>
+        <v>100000</v>
       </c>
       <c r="I3" t="n">
+        <v>1</v>
+      </c>
+      <c r="J3" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>EX</t>
+          <t>RO</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -1869,31 +1884,36 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
+          <t>EX</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
           <t>NONE</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="F4" t="inlineStr">
         <is>
           <t>0.60-0.649</t>
         </is>
       </c>
-      <c r="F4" t="n">
+      <c r="G4" t="n">
         <v>5.4</v>
       </c>
-      <c r="G4" t="n">
-        <v>100000</v>
-      </c>
       <c r="H4" t="n">
-        <v>1</v>
+        <v>100000</v>
       </c>
       <c r="I4" t="n">
+        <v>1</v>
+      </c>
+      <c r="J4" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>EX</t>
+          <t>RO</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -1908,31 +1928,36 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
+          <t>EX</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
           <t>FAINT</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
+      <c r="F5" t="inlineStr">
         <is>
           <t>0.60-0.649</t>
         </is>
       </c>
-      <c r="F5" t="n">
+      <c r="G5" t="n">
         <v>5.4</v>
       </c>
-      <c r="G5" t="n">
-        <v>100000</v>
-      </c>
       <c r="H5" t="n">
-        <v>1</v>
+        <v>100000</v>
       </c>
       <c r="I5" t="n">
+        <v>1</v>
+      </c>
+      <c r="J5" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>EX</t>
+          <t>RO</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -1947,31 +1972,36 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
+          <t>EX</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
           <t>NONE</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
+      <c r="F6" t="inlineStr">
         <is>
           <t>0.80-849</t>
         </is>
       </c>
-      <c r="F6" t="n">
+      <c r="G6" t="n">
         <v>6</v>
       </c>
-      <c r="G6" t="n">
-        <v>100000</v>
-      </c>
       <c r="H6" t="n">
-        <v>1</v>
+        <v>100000</v>
       </c>
       <c r="I6" t="n">
+        <v>1</v>
+      </c>
+      <c r="J6" t="n">
         <v>16</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>EX</t>
+          <t>RO</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -1986,31 +2016,36 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
+          <t>EX</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
           <t>FAINT</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
+      <c r="F7" t="inlineStr">
         <is>
           <t>0.80-849</t>
         </is>
       </c>
-      <c r="F7" t="n">
+      <c r="G7" t="n">
         <v>6</v>
       </c>
-      <c r="G7" t="n">
-        <v>100000</v>
-      </c>
       <c r="H7" t="n">
-        <v>1</v>
+        <v>100000</v>
       </c>
       <c r="I7" t="n">
+        <v>1</v>
+      </c>
+      <c r="J7" t="n">
         <v>16</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>EX</t>
+          <t>RO</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -2025,31 +2060,36 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
+          <t>EX</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
           <t>NONE</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
+      <c r="F8" t="inlineStr">
         <is>
           <t>0.95-0.999</t>
         </is>
       </c>
-      <c r="F8" t="n">
+      <c r="G8" t="n">
         <v>6.3</v>
       </c>
-      <c r="G8" t="n">
-        <v>100000</v>
-      </c>
       <c r="H8" t="n">
-        <v>1</v>
+        <v>100000</v>
       </c>
       <c r="I8" t="n">
+        <v>1</v>
+      </c>
+      <c r="J8" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>EX</t>
+          <t>RO</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -2064,31 +2104,36 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
+          <t>EX</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
           <t>FAINT</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr">
+      <c r="F9" t="inlineStr">
         <is>
           <t>0.95-0.999</t>
         </is>
       </c>
-      <c r="F9" t="n">
+      <c r="G9" t="n">
         <v>6.3</v>
       </c>
-      <c r="G9" t="n">
-        <v>100000</v>
-      </c>
       <c r="H9" t="n">
-        <v>1</v>
+        <v>100000</v>
       </c>
       <c r="I9" t="n">
+        <v>1</v>
+      </c>
+      <c r="J9" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>EX</t>
+          <t>RO</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -2103,31 +2148,36 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
+          <t>EX</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
           <t>NONE</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr">
+      <c r="F10" t="inlineStr">
         <is>
           <t>0.35-0.399</t>
         </is>
       </c>
-      <c r="F10" t="n">
+      <c r="G10" t="n">
         <v>4.5</v>
       </c>
-      <c r="G10" t="n">
-        <v>100000</v>
-      </c>
       <c r="H10" t="n">
-        <v>1</v>
+        <v>100000</v>
       </c>
       <c r="I10" t="n">
+        <v>1</v>
+      </c>
+      <c r="J10" t="n">
         <v>14</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>EX</t>
+          <t>RO</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -2142,31 +2192,36 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
+          <t>EX</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
           <t>FAINT</t>
         </is>
       </c>
-      <c r="E11" t="inlineStr">
+      <c r="F11" t="inlineStr">
         <is>
           <t>0.35-0.399</t>
         </is>
       </c>
-      <c r="F11" t="n">
+      <c r="G11" t="n">
         <v>4.5</v>
       </c>
-      <c r="G11" t="n">
-        <v>100000</v>
-      </c>
       <c r="H11" t="n">
-        <v>1</v>
+        <v>100000</v>
       </c>
       <c r="I11" t="n">
+        <v>1</v>
+      </c>
+      <c r="J11" t="n">
         <v>14</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>EX</t>
+          <t>RO</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -2181,31 +2236,36 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
+          <t>EX</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
           <t>NONE</t>
         </is>
       </c>
-      <c r="E12" t="inlineStr">
+      <c r="F12" t="inlineStr">
         <is>
           <t>0.60-0.649</t>
         </is>
       </c>
-      <c r="F12" t="n">
+      <c r="G12" t="n">
         <v>5.4</v>
       </c>
-      <c r="G12" t="n">
-        <v>100000</v>
-      </c>
       <c r="H12" t="n">
-        <v>1</v>
+        <v>100000</v>
       </c>
       <c r="I12" t="n">
+        <v>1</v>
+      </c>
+      <c r="J12" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>EX</t>
+          <t>RO</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -2220,31 +2280,36 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
+          <t>EX</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
           <t>FAINT</t>
         </is>
       </c>
-      <c r="E13" t="inlineStr">
+      <c r="F13" t="inlineStr">
         <is>
           <t>0.60-0.649</t>
         </is>
       </c>
-      <c r="F13" t="n">
+      <c r="G13" t="n">
         <v>5.4</v>
       </c>
-      <c r="G13" t="n">
-        <v>100000</v>
-      </c>
       <c r="H13" t="n">
-        <v>1</v>
+        <v>100000</v>
       </c>
       <c r="I13" t="n">
+        <v>1</v>
+      </c>
+      <c r="J13" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>EX</t>
+          <t>RO</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -2259,31 +2324,36 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
+          <t>EX</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
           <t>NONE</t>
         </is>
       </c>
-      <c r="E14" t="inlineStr">
+      <c r="F14" t="inlineStr">
         <is>
           <t>0.80-849</t>
         </is>
       </c>
-      <c r="F14" t="n">
+      <c r="G14" t="n">
         <v>6</v>
       </c>
-      <c r="G14" t="n">
-        <v>100000</v>
-      </c>
       <c r="H14" t="n">
-        <v>1</v>
+        <v>100000</v>
       </c>
       <c r="I14" t="n">
+        <v>1</v>
+      </c>
+      <c r="J14" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>EX</t>
+          <t>RO</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -2298,31 +2368,36 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
+          <t>EX</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
           <t>FAINT</t>
         </is>
       </c>
-      <c r="E15" t="inlineStr">
+      <c r="F15" t="inlineStr">
         <is>
           <t>0.80-849</t>
         </is>
       </c>
-      <c r="F15" t="n">
+      <c r="G15" t="n">
         <v>6</v>
       </c>
-      <c r="G15" t="n">
-        <v>100000</v>
-      </c>
       <c r="H15" t="n">
-        <v>1</v>
+        <v>100000</v>
       </c>
       <c r="I15" t="n">
+        <v>1</v>
+      </c>
+      <c r="J15" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>EX</t>
+          <t>RO</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -2337,31 +2412,36 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
+          <t>EX</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
           <t>NONE</t>
         </is>
       </c>
-      <c r="E16" t="inlineStr">
+      <c r="F16" t="inlineStr">
         <is>
           <t>0.95-0.999</t>
         </is>
       </c>
-      <c r="F16" t="n">
+      <c r="G16" t="n">
         <v>6.3</v>
       </c>
-      <c r="G16" t="n">
-        <v>100000</v>
-      </c>
       <c r="H16" t="n">
-        <v>1</v>
+        <v>100000</v>
       </c>
       <c r="I16" t="n">
+        <v>1</v>
+      </c>
+      <c r="J16" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>EX</t>
+          <t>RO</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -2376,31 +2456,36 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
+          <t>EX</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
           <t>FAINT</t>
         </is>
       </c>
-      <c r="E17" t="inlineStr">
+      <c r="F17" t="inlineStr">
         <is>
           <t>0.95-0.999</t>
         </is>
       </c>
-      <c r="F17" t="n">
+      <c r="G17" t="n">
         <v>6.3</v>
       </c>
-      <c r="G17" t="n">
-        <v>100000</v>
-      </c>
       <c r="H17" t="n">
-        <v>1</v>
+        <v>100000</v>
       </c>
       <c r="I17" t="n">
+        <v>1</v>
+      </c>
+      <c r="J17" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>EX</t>
+          <t>RO</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -2415,31 +2500,36 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
+          <t>EX</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
           <t>NONE</t>
         </is>
       </c>
-      <c r="E18" t="inlineStr">
+      <c r="F18" t="inlineStr">
         <is>
           <t>0.35-0.399</t>
         </is>
       </c>
-      <c r="F18" t="n">
+      <c r="G18" t="n">
         <v>4.5</v>
       </c>
-      <c r="G18" t="n">
-        <v>100000</v>
-      </c>
       <c r="H18" t="n">
-        <v>1</v>
+        <v>100000</v>
       </c>
       <c r="I18" t="n">
+        <v>1</v>
+      </c>
+      <c r="J18" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>EX</t>
+          <t>RO</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -2454,31 +2544,36 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
+          <t>EX</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
           <t>FAINT</t>
         </is>
       </c>
-      <c r="E19" t="inlineStr">
+      <c r="F19" t="inlineStr">
         <is>
           <t>0.35-0.399</t>
         </is>
       </c>
-      <c r="F19" t="n">
+      <c r="G19" t="n">
         <v>4.5</v>
       </c>
-      <c r="G19" t="n">
-        <v>100000</v>
-      </c>
       <c r="H19" t="n">
-        <v>1</v>
+        <v>100000</v>
       </c>
       <c r="I19" t="n">
+        <v>1</v>
+      </c>
+      <c r="J19" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>EX</t>
+          <t>RO</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -2493,31 +2588,36 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
+          <t>EX</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
           <t>NONE</t>
         </is>
       </c>
-      <c r="E20" t="inlineStr">
+      <c r="F20" t="inlineStr">
         <is>
           <t>0.60-0.649</t>
         </is>
       </c>
-      <c r="F20" t="n">
+      <c r="G20" t="n">
         <v>5.4</v>
       </c>
-      <c r="G20" t="n">
-        <v>100000</v>
-      </c>
       <c r="H20" t="n">
-        <v>1</v>
+        <v>100000</v>
       </c>
       <c r="I20" t="n">
+        <v>1</v>
+      </c>
+      <c r="J20" t="n">
         <v>7</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>EX</t>
+          <t>RO</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -2532,31 +2632,36 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
+          <t>EX</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
           <t>FAINT</t>
         </is>
       </c>
-      <c r="E21" t="inlineStr">
+      <c r="F21" t="inlineStr">
         <is>
           <t>0.60-0.649</t>
         </is>
       </c>
-      <c r="F21" t="n">
+      <c r="G21" t="n">
         <v>5.4</v>
       </c>
-      <c r="G21" t="n">
-        <v>100000</v>
-      </c>
       <c r="H21" t="n">
-        <v>1</v>
+        <v>100000</v>
       </c>
       <c r="I21" t="n">
+        <v>1</v>
+      </c>
+      <c r="J21" t="n">
         <v>7</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>EX</t>
+          <t>RO</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -2571,31 +2676,36 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
+          <t>EX</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
           <t>NONE</t>
         </is>
       </c>
-      <c r="E22" t="inlineStr">
+      <c r="F22" t="inlineStr">
         <is>
           <t>0.80-849</t>
         </is>
       </c>
-      <c r="F22" t="n">
+      <c r="G22" t="n">
         <v>6</v>
       </c>
-      <c r="G22" t="n">
-        <v>100000</v>
-      </c>
       <c r="H22" t="n">
-        <v>1</v>
+        <v>100000</v>
       </c>
       <c r="I22" t="n">
+        <v>1</v>
+      </c>
+      <c r="J22" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>EX</t>
+          <t>RO</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -2610,31 +2720,36 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
+          <t>EX</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
           <t>FAINT</t>
         </is>
       </c>
-      <c r="E23" t="inlineStr">
+      <c r="F23" t="inlineStr">
         <is>
           <t>0.80-849</t>
         </is>
       </c>
-      <c r="F23" t="n">
+      <c r="G23" t="n">
         <v>6</v>
       </c>
-      <c r="G23" t="n">
-        <v>100000</v>
-      </c>
       <c r="H23" t="n">
-        <v>1</v>
+        <v>100000</v>
       </c>
       <c r="I23" t="n">
+        <v>1</v>
+      </c>
+      <c r="J23" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>EX</t>
+          <t>RO</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -2649,31 +2764,36 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
+          <t>EX</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
           <t>NONE</t>
         </is>
       </c>
-      <c r="E24" t="inlineStr">
+      <c r="F24" t="inlineStr">
         <is>
           <t>0.95-0.999</t>
         </is>
       </c>
-      <c r="F24" t="n">
+      <c r="G24" t="n">
         <v>6.3</v>
       </c>
-      <c r="G24" t="n">
-        <v>100000</v>
-      </c>
       <c r="H24" t="n">
-        <v>1</v>
+        <v>100000</v>
       </c>
       <c r="I24" t="n">
+        <v>1</v>
+      </c>
+      <c r="J24" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>EX</t>
+          <t>RO</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -2688,31 +2808,36 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
+          <t>EX</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
           <t>FAINT</t>
         </is>
       </c>
-      <c r="E25" t="inlineStr">
+      <c r="F25" t="inlineStr">
         <is>
           <t>0.95-0.999</t>
         </is>
       </c>
-      <c r="F25" t="n">
+      <c r="G25" t="n">
         <v>6.3</v>
       </c>
-      <c r="G25" t="n">
-        <v>100000</v>
-      </c>
       <c r="H25" t="n">
-        <v>1</v>
+        <v>100000</v>
       </c>
       <c r="I25" t="n">
+        <v>1</v>
+      </c>
+      <c r="J25" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>EX</t>
+          <t>RO</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -2727,31 +2852,36 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
+          <t>EX</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
           <t>NONE</t>
         </is>
       </c>
-      <c r="E26" t="inlineStr">
+      <c r="F26" t="inlineStr">
         <is>
           <t>0.35-0.399</t>
         </is>
       </c>
-      <c r="F26" t="n">
+      <c r="G26" t="n">
         <v>4.5</v>
       </c>
-      <c r="G26" t="n">
-        <v>100000</v>
-      </c>
       <c r="H26" t="n">
-        <v>1</v>
+        <v>100000</v>
       </c>
       <c r="I26" t="n">
+        <v>1</v>
+      </c>
+      <c r="J26" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>EX</t>
+          <t>RO</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -2766,31 +2896,36 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
+          <t>EX</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
           <t>FAINT</t>
         </is>
       </c>
-      <c r="E27" t="inlineStr">
+      <c r="F27" t="inlineStr">
         <is>
           <t>0.35-0.399</t>
         </is>
       </c>
-      <c r="F27" t="n">
+      <c r="G27" t="n">
         <v>4.5</v>
       </c>
-      <c r="G27" t="n">
-        <v>100000</v>
-      </c>
       <c r="H27" t="n">
-        <v>1</v>
+        <v>100000</v>
       </c>
       <c r="I27" t="n">
+        <v>1</v>
+      </c>
+      <c r="J27" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>EX</t>
+          <t>RO</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -2805,31 +2940,36 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
+          <t>EX</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
           <t>NONE</t>
         </is>
       </c>
-      <c r="E28" t="inlineStr">
+      <c r="F28" t="inlineStr">
         <is>
           <t>0.60-0.649</t>
         </is>
       </c>
-      <c r="F28" t="n">
+      <c r="G28" t="n">
         <v>5.4</v>
       </c>
-      <c r="G28" t="n">
-        <v>100000</v>
-      </c>
       <c r="H28" t="n">
-        <v>1</v>
+        <v>100000</v>
       </c>
       <c r="I28" t="n">
+        <v>1</v>
+      </c>
+      <c r="J28" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>EX</t>
+          <t>RO</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -2844,31 +2984,36 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
+          <t>EX</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
           <t>FAINT</t>
         </is>
       </c>
-      <c r="E29" t="inlineStr">
+      <c r="F29" t="inlineStr">
         <is>
           <t>0.60-0.649</t>
         </is>
       </c>
-      <c r="F29" t="n">
+      <c r="G29" t="n">
         <v>5.4</v>
       </c>
-      <c r="G29" t="n">
-        <v>100000</v>
-      </c>
       <c r="H29" t="n">
-        <v>1</v>
+        <v>100000</v>
       </c>
       <c r="I29" t="n">
+        <v>1</v>
+      </c>
+      <c r="J29" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>EX</t>
+          <t>RO</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -2883,31 +3028,36 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
+          <t>EX</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
           <t>NONE</t>
         </is>
       </c>
-      <c r="E30" t="inlineStr">
+      <c r="F30" t="inlineStr">
         <is>
           <t>0.80-849</t>
         </is>
       </c>
-      <c r="F30" t="n">
+      <c r="G30" t="n">
         <v>6</v>
       </c>
-      <c r="G30" t="n">
-        <v>100000</v>
-      </c>
       <c r="H30" t="n">
-        <v>1</v>
+        <v>100000</v>
       </c>
       <c r="I30" t="n">
+        <v>1</v>
+      </c>
+      <c r="J30" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>EX</t>
+          <t>RO</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -2922,31 +3072,36 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
+          <t>EX</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
           <t>FAINT</t>
         </is>
       </c>
-      <c r="E31" t="inlineStr">
+      <c r="F31" t="inlineStr">
         <is>
           <t>0.80-849</t>
         </is>
       </c>
-      <c r="F31" t="n">
+      <c r="G31" t="n">
         <v>6</v>
       </c>
-      <c r="G31" t="n">
-        <v>100000</v>
-      </c>
       <c r="H31" t="n">
-        <v>1</v>
+        <v>100000</v>
       </c>
       <c r="I31" t="n">
+        <v>1</v>
+      </c>
+      <c r="J31" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>EX</t>
+          <t>RO</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -2961,31 +3116,36 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
+          <t>EX</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
           <t>NONE</t>
         </is>
       </c>
-      <c r="E32" t="inlineStr">
+      <c r="F32" t="inlineStr">
         <is>
           <t>0.95-0.999</t>
         </is>
       </c>
-      <c r="F32" t="n">
+      <c r="G32" t="n">
         <v>6.3</v>
       </c>
-      <c r="G32" t="n">
-        <v>100000</v>
-      </c>
       <c r="H32" t="n">
-        <v>1</v>
+        <v>100000</v>
       </c>
       <c r="I32" t="n">
+        <v>1</v>
+      </c>
+      <c r="J32" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>EX</t>
+          <t>RO</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -3000,31 +3160,36 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
+          <t>EX</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
           <t>FAINT</t>
         </is>
       </c>
-      <c r="E33" t="inlineStr">
+      <c r="F33" t="inlineStr">
         <is>
           <t>0.95-0.999</t>
         </is>
       </c>
-      <c r="F33" t="n">
+      <c r="G33" t="n">
         <v>6.3</v>
       </c>
-      <c r="G33" t="n">
-        <v>100000</v>
-      </c>
       <c r="H33" t="n">
-        <v>1</v>
+        <v>100000</v>
       </c>
       <c r="I33" t="n">
+        <v>1</v>
+      </c>
+      <c r="J33" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>EX</t>
+          <t>RO</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -3039,31 +3204,36 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
+          <t>EX</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
           <t>NONE</t>
         </is>
       </c>
-      <c r="E34" t="inlineStr">
+      <c r="F34" t="inlineStr">
         <is>
           <t>0.35-0.399</t>
         </is>
       </c>
-      <c r="F34" t="n">
+      <c r="G34" t="n">
         <v>4.5</v>
       </c>
-      <c r="G34" t="n">
-        <v>100000</v>
-      </c>
       <c r="H34" t="n">
-        <v>1</v>
+        <v>100000</v>
       </c>
       <c r="I34" t="n">
+        <v>1</v>
+      </c>
+      <c r="J34" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>EX</t>
+          <t>RO</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -3078,31 +3248,36 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
+          <t>EX</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
           <t>FAINT</t>
         </is>
       </c>
-      <c r="E35" t="inlineStr">
+      <c r="F35" t="inlineStr">
         <is>
           <t>0.35-0.399</t>
         </is>
       </c>
-      <c r="F35" t="n">
+      <c r="G35" t="n">
         <v>4.5</v>
       </c>
-      <c r="G35" t="n">
-        <v>100000</v>
-      </c>
       <c r="H35" t="n">
-        <v>1</v>
+        <v>100000</v>
       </c>
       <c r="I35" t="n">
+        <v>1</v>
+      </c>
+      <c r="J35" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>EX</t>
+          <t>RO</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -3117,31 +3292,36 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
+          <t>EX</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
           <t>NONE</t>
         </is>
       </c>
-      <c r="E36" t="inlineStr">
+      <c r="F36" t="inlineStr">
         <is>
           <t>0.60-0.649</t>
         </is>
       </c>
-      <c r="F36" t="n">
+      <c r="G36" t="n">
         <v>5.4</v>
       </c>
-      <c r="G36" t="n">
-        <v>100000</v>
-      </c>
       <c r="H36" t="n">
-        <v>1</v>
+        <v>100000</v>
       </c>
       <c r="I36" t="n">
+        <v>1</v>
+      </c>
+      <c r="J36" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>EX</t>
+          <t>RO</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -3156,31 +3336,36 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
+          <t>EX</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
           <t>FAINT</t>
         </is>
       </c>
-      <c r="E37" t="inlineStr">
+      <c r="F37" t="inlineStr">
         <is>
           <t>0.60-0.649</t>
         </is>
       </c>
-      <c r="F37" t="n">
+      <c r="G37" t="n">
         <v>5.4</v>
       </c>
-      <c r="G37" t="n">
-        <v>100000</v>
-      </c>
       <c r="H37" t="n">
-        <v>1</v>
+        <v>100000</v>
       </c>
       <c r="I37" t="n">
+        <v>1</v>
+      </c>
+      <c r="J37" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>EX</t>
+          <t>RO</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -3195,31 +3380,36 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
+          <t>EX</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
           <t>NONE</t>
         </is>
       </c>
-      <c r="E38" t="inlineStr">
+      <c r="F38" t="inlineStr">
         <is>
           <t>0.80-849</t>
         </is>
       </c>
-      <c r="F38" t="n">
+      <c r="G38" t="n">
         <v>6</v>
       </c>
-      <c r="G38" t="n">
-        <v>100000</v>
-      </c>
       <c r="H38" t="n">
-        <v>1</v>
+        <v>100000</v>
       </c>
       <c r="I38" t="n">
+        <v>1</v>
+      </c>
+      <c r="J38" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>EX</t>
+          <t>RO</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -3234,31 +3424,36 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
+          <t>EX</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
           <t>FAINT</t>
         </is>
       </c>
-      <c r="E39" t="inlineStr">
+      <c r="F39" t="inlineStr">
         <is>
           <t>0.80-849</t>
         </is>
       </c>
-      <c r="F39" t="n">
+      <c r="G39" t="n">
         <v>6</v>
       </c>
-      <c r="G39" t="n">
-        <v>100000</v>
-      </c>
       <c r="H39" t="n">
-        <v>1</v>
+        <v>100000</v>
       </c>
       <c r="I39" t="n">
+        <v>1</v>
+      </c>
+      <c r="J39" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>EX</t>
+          <t>RO</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -3273,31 +3468,36 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
+          <t>EX</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
           <t>NONE</t>
         </is>
       </c>
-      <c r="E40" t="inlineStr">
+      <c r="F40" t="inlineStr">
         <is>
           <t>0.95-0.999</t>
         </is>
       </c>
-      <c r="F40" t="n">
+      <c r="G40" t="n">
         <v>6.3</v>
       </c>
-      <c r="G40" t="n">
-        <v>100000</v>
-      </c>
       <c r="H40" t="n">
-        <v>1</v>
+        <v>100000</v>
       </c>
       <c r="I40" t="n">
+        <v>1</v>
+      </c>
+      <c r="J40" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>EX</t>
+          <t>RO</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -3312,31 +3512,36 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
+          <t>EX</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
           <t>FAINT</t>
         </is>
       </c>
-      <c r="E41" t="inlineStr">
+      <c r="F41" t="inlineStr">
         <is>
           <t>0.95-0.999</t>
         </is>
       </c>
-      <c r="F41" t="n">
+      <c r="G41" t="n">
         <v>6.3</v>
       </c>
-      <c r="G41" t="n">
-        <v>100000</v>
-      </c>
       <c r="H41" t="n">
-        <v>1</v>
+        <v>100000</v>
       </c>
       <c r="I41" t="n">
+        <v>1</v>
+      </c>
+      <c r="J41" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>EX</t>
+          <t>RO</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -3351,31 +3556,36 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
+          <t>EX</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
           <t>NONE</t>
         </is>
       </c>
-      <c r="E42" t="inlineStr">
+      <c r="F42" t="inlineStr">
         <is>
           <t>0.35-0.399</t>
         </is>
       </c>
-      <c r="F42" t="n">
+      <c r="G42" t="n">
         <v>4.5</v>
       </c>
-      <c r="G42" t="n">
-        <v>100000</v>
-      </c>
       <c r="H42" t="n">
-        <v>1</v>
+        <v>100000</v>
       </c>
       <c r="I42" t="n">
+        <v>1</v>
+      </c>
+      <c r="J42" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>EX</t>
+          <t>RO</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -3390,31 +3600,36 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
+          <t>EX</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
           <t>FAINT</t>
         </is>
       </c>
-      <c r="E43" t="inlineStr">
+      <c r="F43" t="inlineStr">
         <is>
           <t>0.35-0.399</t>
         </is>
       </c>
-      <c r="F43" t="n">
+      <c r="G43" t="n">
         <v>4.5</v>
       </c>
-      <c r="G43" t="n">
-        <v>100000</v>
-      </c>
       <c r="H43" t="n">
-        <v>1</v>
+        <v>100000</v>
       </c>
       <c r="I43" t="n">
+        <v>1</v>
+      </c>
+      <c r="J43" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>EX</t>
+          <t>RO</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -3429,31 +3644,36 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
+          <t>EX</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
           <t>NONE</t>
         </is>
       </c>
-      <c r="E44" t="inlineStr">
+      <c r="F44" t="inlineStr">
         <is>
           <t>0.60-0.649</t>
         </is>
       </c>
-      <c r="F44" t="n">
+      <c r="G44" t="n">
         <v>5.4</v>
       </c>
-      <c r="G44" t="n">
-        <v>100000</v>
-      </c>
       <c r="H44" t="n">
-        <v>1</v>
+        <v>100000</v>
       </c>
       <c r="I44" t="n">
+        <v>1</v>
+      </c>
+      <c r="J44" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>EX</t>
+          <t>RO</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -3468,31 +3688,36 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
+          <t>EX</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
           <t>FAINT</t>
         </is>
       </c>
-      <c r="E45" t="inlineStr">
+      <c r="F45" t="inlineStr">
         <is>
           <t>0.60-0.649</t>
         </is>
       </c>
-      <c r="F45" t="n">
+      <c r="G45" t="n">
         <v>5.4</v>
       </c>
-      <c r="G45" t="n">
-        <v>100000</v>
-      </c>
       <c r="H45" t="n">
-        <v>1</v>
+        <v>100000</v>
       </c>
       <c r="I45" t="n">
+        <v>1</v>
+      </c>
+      <c r="J45" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>EX</t>
+          <t>RO</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -3507,31 +3732,36 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
+          <t>EX</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
           <t>NONE</t>
         </is>
       </c>
-      <c r="E46" t="inlineStr">
+      <c r="F46" t="inlineStr">
         <is>
           <t>0.80-849</t>
         </is>
       </c>
-      <c r="F46" t="n">
+      <c r="G46" t="n">
         <v>6</v>
       </c>
-      <c r="G46" t="n">
-        <v>100000</v>
-      </c>
       <c r="H46" t="n">
-        <v>1</v>
+        <v>100000</v>
       </c>
       <c r="I46" t="n">
+        <v>1</v>
+      </c>
+      <c r="J46" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>EX</t>
+          <t>RO</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -3546,31 +3776,36 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
+          <t>EX</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
           <t>FAINT</t>
         </is>
       </c>
-      <c r="E47" t="inlineStr">
+      <c r="F47" t="inlineStr">
         <is>
           <t>0.80-849</t>
         </is>
       </c>
-      <c r="F47" t="n">
+      <c r="G47" t="n">
         <v>6</v>
       </c>
-      <c r="G47" t="n">
-        <v>100000</v>
-      </c>
       <c r="H47" t="n">
-        <v>1</v>
+        <v>100000</v>
       </c>
       <c r="I47" t="n">
+        <v>1</v>
+      </c>
+      <c r="J47" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>EX</t>
+          <t>RO</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -3585,31 +3820,36 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
+          <t>EX</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
           <t>NONE</t>
         </is>
       </c>
-      <c r="E48" t="inlineStr">
+      <c r="F48" t="inlineStr">
         <is>
           <t>0.95-0.999</t>
         </is>
       </c>
-      <c r="F48" t="n">
+      <c r="G48" t="n">
         <v>6.3</v>
       </c>
-      <c r="G48" t="n">
-        <v>100000</v>
-      </c>
       <c r="H48" t="n">
-        <v>1</v>
+        <v>100000</v>
       </c>
       <c r="I48" t="n">
+        <v>1</v>
+      </c>
+      <c r="J48" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>EX</t>
+          <t>RO</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -3624,1140 +3864,1325 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
+          <t>EX</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
           <t>FAINT</t>
         </is>
       </c>
-      <c r="E49" t="inlineStr">
+      <c r="F49" t="inlineStr">
         <is>
           <t>0.95-0.999</t>
         </is>
       </c>
-      <c r="F49" t="n">
+      <c r="G49" t="n">
         <v>6.3</v>
       </c>
-      <c r="G49" t="n">
-        <v>100000</v>
-      </c>
       <c r="H49" t="n">
-        <v>1</v>
+        <v>100000</v>
       </c>
       <c r="I49" t="n">
+        <v>1</v>
+      </c>
+      <c r="J49" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
+          <t>RO</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
           <t>VG</t>
         </is>
       </c>
-      <c r="B50" t="inlineStr"/>
       <c r="C50" t="inlineStr"/>
-      <c r="D50" t="inlineStr">
+      <c r="D50" t="inlineStr"/>
+      <c r="E50" t="inlineStr">
         <is>
           <t>NONE</t>
         </is>
       </c>
-      <c r="E50" t="inlineStr">
+      <c r="F50" t="inlineStr">
         <is>
           <t>1.00-1.49</t>
         </is>
       </c>
-      <c r="F50" t="n">
+      <c r="G50" t="n">
         <v>0</v>
       </c>
-      <c r="G50" t="n">
+      <c r="H50" t="n">
         <v>6.2</v>
       </c>
-      <c r="H50" t="n">
-        <v>1</v>
-      </c>
       <c r="I50" t="n">
+        <v>1</v>
+      </c>
+      <c r="J50" t="n">
         <v>-0.5</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
+          <t>RO</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
           <t>VG</t>
         </is>
       </c>
-      <c r="B51" t="inlineStr"/>
       <c r="C51" t="inlineStr"/>
-      <c r="D51" t="inlineStr">
+      <c r="D51" t="inlineStr"/>
+      <c r="E51" t="inlineStr">
         <is>
           <t>FAINT</t>
         </is>
       </c>
-      <c r="E51" t="inlineStr">
+      <c r="F51" t="inlineStr">
         <is>
           <t>1.00-1.49</t>
         </is>
       </c>
-      <c r="F51" t="n">
+      <c r="G51" t="n">
         <v>0</v>
       </c>
-      <c r="G51" t="n">
+      <c r="H51" t="n">
         <v>6.2</v>
       </c>
-      <c r="H51" t="n">
-        <v>1</v>
-      </c>
       <c r="I51" t="n">
+        <v>1</v>
+      </c>
+      <c r="J51" t="n">
         <v>-0.5</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
+          <t>RO</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
           <t>VG</t>
         </is>
       </c>
-      <c r="B52" t="inlineStr"/>
       <c r="C52" t="inlineStr"/>
-      <c r="D52" t="inlineStr">
+      <c r="D52" t="inlineStr"/>
+      <c r="E52" t="inlineStr">
         <is>
           <t>NONE</t>
         </is>
       </c>
-      <c r="E52" t="inlineStr">
+      <c r="F52" t="inlineStr">
         <is>
           <t>1.00-1.49</t>
         </is>
       </c>
-      <c r="F52" t="n">
+      <c r="G52" t="n">
         <v>0</v>
       </c>
-      <c r="G52" t="n">
+      <c r="H52" t="n">
         <v>6.2</v>
       </c>
-      <c r="H52" t="n">
+      <c r="I52" t="n">
         <v>2</v>
       </c>
-      <c r="I52" t="n">
+      <c r="J52" t="n">
         <v>-0.5</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
+          <t>RO</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
           <t>VG</t>
         </is>
       </c>
-      <c r="B53" t="inlineStr"/>
       <c r="C53" t="inlineStr"/>
-      <c r="D53" t="inlineStr">
+      <c r="D53" t="inlineStr"/>
+      <c r="E53" t="inlineStr">
         <is>
           <t>FAINT</t>
         </is>
       </c>
-      <c r="E53" t="inlineStr">
+      <c r="F53" t="inlineStr">
         <is>
           <t>1.00-1.49</t>
         </is>
       </c>
-      <c r="F53" t="n">
+      <c r="G53" t="n">
         <v>0</v>
       </c>
-      <c r="G53" t="n">
+      <c r="H53" t="n">
         <v>6.2</v>
       </c>
-      <c r="H53" t="n">
+      <c r="I53" t="n">
         <v>2</v>
       </c>
-      <c r="I53" t="n">
+      <c r="J53" t="n">
         <v>-0.5</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
+          <t>RO</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
           <t>VG</t>
         </is>
       </c>
-      <c r="B54" t="inlineStr"/>
       <c r="C54" t="inlineStr"/>
-      <c r="D54" t="inlineStr">
+      <c r="D54" t="inlineStr"/>
+      <c r="E54" t="inlineStr">
         <is>
           <t>NONE</t>
         </is>
       </c>
-      <c r="E54" t="inlineStr">
+      <c r="F54" t="inlineStr">
         <is>
           <t>1.00-1.49</t>
         </is>
       </c>
-      <c r="F54" t="n">
+      <c r="G54" t="n">
         <v>0</v>
       </c>
-      <c r="G54" t="n">
+      <c r="H54" t="n">
         <v>6.2</v>
       </c>
-      <c r="H54" t="n">
+      <c r="I54" t="n">
         <v>3</v>
       </c>
-      <c r="I54" t="n">
+      <c r="J54" t="n">
         <v>-0.5</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
+          <t>RO</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
           <t>VG</t>
         </is>
       </c>
-      <c r="B55" t="inlineStr"/>
       <c r="C55" t="inlineStr"/>
-      <c r="D55" t="inlineStr">
+      <c r="D55" t="inlineStr"/>
+      <c r="E55" t="inlineStr">
         <is>
           <t>FAINT</t>
         </is>
       </c>
-      <c r="E55" t="inlineStr">
+      <c r="F55" t="inlineStr">
         <is>
           <t>1.00-1.49</t>
         </is>
       </c>
-      <c r="F55" t="n">
+      <c r="G55" t="n">
         <v>0</v>
       </c>
-      <c r="G55" t="n">
+      <c r="H55" t="n">
         <v>6.2</v>
       </c>
-      <c r="H55" t="n">
+      <c r="I55" t="n">
         <v>3</v>
       </c>
-      <c r="I55" t="n">
+      <c r="J55" t="n">
         <v>-0.5</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
+          <t>RO</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
           <t>VG</t>
         </is>
       </c>
-      <c r="B56" t="inlineStr"/>
       <c r="C56" t="inlineStr"/>
-      <c r="D56" t="inlineStr">
+      <c r="D56" t="inlineStr"/>
+      <c r="E56" t="inlineStr">
         <is>
           <t>NONE</t>
         </is>
       </c>
-      <c r="E56" t="inlineStr">
+      <c r="F56" t="inlineStr">
         <is>
           <t>1.00-1.49</t>
         </is>
       </c>
-      <c r="F56" t="n">
+      <c r="G56" t="n">
         <v>0</v>
       </c>
-      <c r="G56" t="n">
+      <c r="H56" t="n">
         <v>6.2</v>
       </c>
-      <c r="H56" t="n">
+      <c r="I56" t="n">
         <v>4</v>
       </c>
-      <c r="I56" t="n">
+      <c r="J56" t="n">
         <v>-0.5</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
+          <t>RO</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
           <t>VG</t>
         </is>
       </c>
-      <c r="B57" t="inlineStr"/>
       <c r="C57" t="inlineStr"/>
-      <c r="D57" t="inlineStr">
+      <c r="D57" t="inlineStr"/>
+      <c r="E57" t="inlineStr">
         <is>
           <t>FAINT</t>
         </is>
       </c>
-      <c r="E57" t="inlineStr">
+      <c r="F57" t="inlineStr">
         <is>
           <t>1.00-1.49</t>
         </is>
       </c>
-      <c r="F57" t="n">
+      <c r="G57" t="n">
         <v>0</v>
       </c>
-      <c r="G57" t="n">
+      <c r="H57" t="n">
         <v>6.2</v>
       </c>
-      <c r="H57" t="n">
+      <c r="I57" t="n">
         <v>4</v>
       </c>
-      <c r="I57" t="n">
+      <c r="J57" t="n">
         <v>-0.5</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
+          <t>RO</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
           <t>VG</t>
         </is>
       </c>
-      <c r="B58" t="inlineStr"/>
       <c r="C58" t="inlineStr"/>
-      <c r="D58" t="inlineStr">
+      <c r="D58" t="inlineStr"/>
+      <c r="E58" t="inlineStr">
         <is>
           <t>NONE</t>
         </is>
       </c>
-      <c r="E58" t="inlineStr">
+      <c r="F58" t="inlineStr">
         <is>
           <t>1.00-1.49</t>
         </is>
       </c>
-      <c r="F58" t="n">
+      <c r="G58" t="n">
         <v>0</v>
       </c>
-      <c r="G58" t="n">
+      <c r="H58" t="n">
         <v>6.2</v>
       </c>
-      <c r="H58" t="n">
+      <c r="I58" t="n">
         <v>5</v>
       </c>
-      <c r="I58" t="n">
+      <c r="J58" t="n">
         <v>-0.05</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
+          <t>RO</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
           <t>VG</t>
         </is>
       </c>
-      <c r="B59" t="inlineStr"/>
       <c r="C59" t="inlineStr"/>
-      <c r="D59" t="inlineStr">
+      <c r="D59" t="inlineStr"/>
+      <c r="E59" t="inlineStr">
         <is>
           <t>FAINT</t>
         </is>
       </c>
-      <c r="E59" t="inlineStr">
+      <c r="F59" t="inlineStr">
         <is>
           <t>1.00-1.49</t>
         </is>
       </c>
-      <c r="F59" t="n">
+      <c r="G59" t="n">
         <v>0</v>
       </c>
-      <c r="G59" t="n">
+      <c r="H59" t="n">
         <v>6.2</v>
       </c>
-      <c r="H59" t="n">
+      <c r="I59" t="n">
         <v>5</v>
       </c>
-      <c r="I59" t="n">
+      <c r="J59" t="n">
         <v>-0.05</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
+          <t>RO</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
           <t>VG</t>
         </is>
       </c>
-      <c r="B60" t="inlineStr"/>
       <c r="C60" t="inlineStr"/>
-      <c r="D60" t="inlineStr">
+      <c r="D60" t="inlineStr"/>
+      <c r="E60" t="inlineStr">
         <is>
           <t>NONE</t>
         </is>
       </c>
-      <c r="E60" t="inlineStr">
+      <c r="F60" t="inlineStr">
         <is>
           <t>1.00-1.49</t>
         </is>
       </c>
-      <c r="F60" t="n">
+      <c r="G60" t="n">
         <v>0</v>
       </c>
-      <c r="G60" t="n">
+      <c r="H60" t="n">
         <v>6.2</v>
       </c>
-      <c r="H60" t="n">
+      <c r="I60" t="n">
         <v>6</v>
       </c>
-      <c r="I60" t="n">
+      <c r="J60" t="n">
         <v>-0.5</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
+          <t>RO</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
           <t>VG</t>
         </is>
       </c>
-      <c r="B61" t="inlineStr"/>
       <c r="C61" t="inlineStr"/>
-      <c r="D61" t="inlineStr">
+      <c r="D61" t="inlineStr"/>
+      <c r="E61" t="inlineStr">
         <is>
           <t>FAINT</t>
         </is>
       </c>
-      <c r="E61" t="inlineStr">
+      <c r="F61" t="inlineStr">
         <is>
           <t>1.00-1.49</t>
         </is>
       </c>
-      <c r="F61" t="n">
+      <c r="G61" t="n">
         <v>0</v>
       </c>
-      <c r="G61" t="n">
+      <c r="H61" t="n">
         <v>6.2</v>
       </c>
-      <c r="H61" t="n">
+      <c r="I61" t="n">
         <v>6</v>
       </c>
-      <c r="I61" t="n">
+      <c r="J61" t="n">
         <v>-0.5</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
+          <t>RO</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
           <t>VG</t>
         </is>
       </c>
-      <c r="B62" t="inlineStr"/>
       <c r="C62" t="inlineStr"/>
-      <c r="D62" t="inlineStr">
+      <c r="D62" t="inlineStr"/>
+      <c r="E62" t="inlineStr">
         <is>
           <t>NONE</t>
         </is>
       </c>
-      <c r="E62" t="inlineStr">
+      <c r="F62" t="inlineStr">
         <is>
           <t>1.00-1.49</t>
         </is>
       </c>
-      <c r="F62" t="n">
+      <c r="G62" t="n">
         <v>0</v>
       </c>
-      <c r="G62" t="n">
+      <c r="H62" t="n">
         <v>6.2</v>
       </c>
-      <c r="H62" t="n">
+      <c r="I62" t="n">
         <v>7</v>
       </c>
-      <c r="I62" t="n">
+      <c r="J62" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
+          <t>RO</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
           <t>VG</t>
         </is>
       </c>
-      <c r="B63" t="inlineStr"/>
       <c r="C63" t="inlineStr"/>
-      <c r="D63" t="inlineStr">
+      <c r="D63" t="inlineStr"/>
+      <c r="E63" t="inlineStr">
         <is>
           <t>FAINT</t>
         </is>
       </c>
-      <c r="E63" t="inlineStr">
+      <c r="F63" t="inlineStr">
         <is>
           <t>1.00-1.49</t>
         </is>
       </c>
-      <c r="F63" t="n">
+      <c r="G63" t="n">
         <v>0</v>
       </c>
-      <c r="G63" t="n">
+      <c r="H63" t="n">
         <v>6.2</v>
       </c>
-      <c r="H63" t="n">
+      <c r="I63" t="n">
         <v>7</v>
       </c>
-      <c r="I63" t="n">
+      <c r="J63" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
+          <t>RO</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
           <t>VG</t>
         </is>
       </c>
-      <c r="B64" t="inlineStr"/>
       <c r="C64" t="inlineStr"/>
-      <c r="D64" t="inlineStr">
+      <c r="D64" t="inlineStr"/>
+      <c r="E64" t="inlineStr">
         <is>
           <t>NONE</t>
         </is>
       </c>
-      <c r="E64" t="inlineStr">
+      <c r="F64" t="inlineStr">
         <is>
           <t>1.00-1.49</t>
         </is>
       </c>
-      <c r="F64" t="n">
+      <c r="G64" t="n">
         <v>0</v>
       </c>
-      <c r="G64" t="n">
+      <c r="H64" t="n">
         <v>6.2</v>
       </c>
-      <c r="H64" t="n">
+      <c r="I64" t="n">
         <v>8</v>
       </c>
-      <c r="I64" t="n">
+      <c r="J64" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
+          <t>RO</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
           <t>VG</t>
         </is>
       </c>
-      <c r="B65" t="inlineStr"/>
       <c r="C65" t="inlineStr"/>
-      <c r="D65" t="inlineStr">
+      <c r="D65" t="inlineStr"/>
+      <c r="E65" t="inlineStr">
         <is>
           <t>FAINT</t>
         </is>
       </c>
-      <c r="E65" t="inlineStr">
+      <c r="F65" t="inlineStr">
         <is>
           <t>1.00-1.49</t>
         </is>
       </c>
-      <c r="F65" t="n">
+      <c r="G65" t="n">
         <v>0</v>
       </c>
-      <c r="G65" t="n">
+      <c r="H65" t="n">
         <v>6.2</v>
       </c>
-      <c r="H65" t="n">
+      <c r="I65" t="n">
         <v>8</v>
       </c>
-      <c r="I65" t="n">
+      <c r="J65" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
+          <t>RO</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
           <t>VG</t>
         </is>
       </c>
-      <c r="B66" t="inlineStr"/>
       <c r="C66" t="inlineStr"/>
-      <c r="D66" t="inlineStr">
+      <c r="D66" t="inlineStr"/>
+      <c r="E66" t="inlineStr">
         <is>
           <t>NONE</t>
         </is>
       </c>
-      <c r="E66" t="inlineStr">
+      <c r="F66" t="inlineStr">
         <is>
           <t>1.00-1.49</t>
         </is>
       </c>
-      <c r="F66" t="n">
+      <c r="G66" t="n">
         <v>0</v>
       </c>
-      <c r="G66" t="n">
+      <c r="H66" t="n">
         <v>6.2</v>
       </c>
-      <c r="H66" t="n">
+      <c r="I66" t="n">
         <v>9</v>
       </c>
-      <c r="I66" t="n">
+      <c r="J66" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
+          <t>RO</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
           <t>VG</t>
         </is>
       </c>
-      <c r="B67" t="inlineStr"/>
       <c r="C67" t="inlineStr"/>
-      <c r="D67" t="inlineStr">
+      <c r="D67" t="inlineStr"/>
+      <c r="E67" t="inlineStr">
         <is>
           <t>FAINT</t>
         </is>
       </c>
-      <c r="E67" t="inlineStr">
+      <c r="F67" t="inlineStr">
         <is>
           <t>1.00-1.49</t>
         </is>
       </c>
-      <c r="F67" t="n">
+      <c r="G67" t="n">
         <v>0</v>
       </c>
-      <c r="G67" t="n">
+      <c r="H67" t="n">
         <v>6.2</v>
       </c>
-      <c r="H67" t="n">
+      <c r="I67" t="n">
         <v>9</v>
       </c>
-      <c r="I67" t="n">
+      <c r="J67" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
+          <t>RO</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
           <t>VG</t>
         </is>
       </c>
-      <c r="B68" t="inlineStr"/>
       <c r="C68" t="inlineStr"/>
-      <c r="D68" t="inlineStr">
+      <c r="D68" t="inlineStr"/>
+      <c r="E68" t="inlineStr">
         <is>
           <t>NONE</t>
         </is>
       </c>
-      <c r="E68" t="inlineStr">
+      <c r="F68" t="inlineStr">
         <is>
           <t>1.00-1.49</t>
         </is>
       </c>
-      <c r="F68" t="n">
+      <c r="G68" t="n">
         <v>6.3</v>
       </c>
-      <c r="G68" t="n">
-        <v>100000</v>
-      </c>
       <c r="H68" t="n">
-        <v>1</v>
+        <v>100000</v>
       </c>
       <c r="I68" t="n">
+        <v>1</v>
+      </c>
+      <c r="J68" t="n">
         <v>1.5</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
+          <t>RO</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
           <t>VG</t>
         </is>
       </c>
-      <c r="B69" t="inlineStr"/>
       <c r="C69" t="inlineStr"/>
-      <c r="D69" t="inlineStr">
+      <c r="D69" t="inlineStr"/>
+      <c r="E69" t="inlineStr">
         <is>
           <t>FAINT</t>
         </is>
       </c>
-      <c r="E69" t="inlineStr">
+      <c r="F69" t="inlineStr">
         <is>
           <t>1.00-1.49</t>
         </is>
       </c>
-      <c r="F69" t="n">
+      <c r="G69" t="n">
         <v>6.3</v>
       </c>
-      <c r="G69" t="n">
-        <v>100000</v>
-      </c>
       <c r="H69" t="n">
-        <v>1</v>
+        <v>100000</v>
       </c>
       <c r="I69" t="n">
+        <v>1</v>
+      </c>
+      <c r="J69" t="n">
         <v>1.5</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
+          <t>RO</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
           <t>VG</t>
         </is>
       </c>
-      <c r="B70" t="inlineStr"/>
       <c r="C70" t="inlineStr"/>
-      <c r="D70" t="inlineStr">
+      <c r="D70" t="inlineStr"/>
+      <c r="E70" t="inlineStr">
         <is>
           <t>NONE</t>
         </is>
       </c>
-      <c r="E70" t="inlineStr">
+      <c r="F70" t="inlineStr">
         <is>
           <t>1.00-1.49</t>
         </is>
       </c>
-      <c r="F70" t="n">
+      <c r="G70" t="n">
         <v>6.3</v>
       </c>
-      <c r="G70" t="n">
-        <v>100000</v>
-      </c>
       <c r="H70" t="n">
+        <v>100000</v>
+      </c>
+      <c r="I70" t="n">
         <v>2</v>
       </c>
-      <c r="I70" t="n">
+      <c r="J70" t="n">
         <v>1.5</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
+          <t>RO</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
           <t>VG</t>
         </is>
       </c>
-      <c r="B71" t="inlineStr"/>
       <c r="C71" t="inlineStr"/>
-      <c r="D71" t="inlineStr">
+      <c r="D71" t="inlineStr"/>
+      <c r="E71" t="inlineStr">
         <is>
           <t>FAINT</t>
         </is>
       </c>
-      <c r="E71" t="inlineStr">
+      <c r="F71" t="inlineStr">
         <is>
           <t>1.00-1.49</t>
         </is>
       </c>
-      <c r="F71" t="n">
+      <c r="G71" t="n">
         <v>6.3</v>
       </c>
-      <c r="G71" t="n">
-        <v>100000</v>
-      </c>
       <c r="H71" t="n">
+        <v>100000</v>
+      </c>
+      <c r="I71" t="n">
         <v>2</v>
       </c>
-      <c r="I71" t="n">
+      <c r="J71" t="n">
         <v>1.5</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
+          <t>RO</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
           <t>VG</t>
         </is>
       </c>
-      <c r="B72" t="inlineStr"/>
       <c r="C72" t="inlineStr"/>
-      <c r="D72" t="inlineStr">
+      <c r="D72" t="inlineStr"/>
+      <c r="E72" t="inlineStr">
         <is>
           <t>NONE</t>
         </is>
       </c>
-      <c r="E72" t="inlineStr">
+      <c r="F72" t="inlineStr">
         <is>
           <t>1.00-1.49</t>
         </is>
       </c>
-      <c r="F72" t="n">
+      <c r="G72" t="n">
         <v>6.3</v>
       </c>
-      <c r="G72" t="n">
-        <v>100000</v>
-      </c>
       <c r="H72" t="n">
+        <v>100000</v>
+      </c>
+      <c r="I72" t="n">
         <v>3</v>
       </c>
-      <c r="I72" t="n">
+      <c r="J72" t="n">
         <v>1.5</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
+          <t>RO</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
           <t>VG</t>
         </is>
       </c>
-      <c r="B73" t="inlineStr"/>
       <c r="C73" t="inlineStr"/>
-      <c r="D73" t="inlineStr">
+      <c r="D73" t="inlineStr"/>
+      <c r="E73" t="inlineStr">
         <is>
           <t>FAINT</t>
         </is>
       </c>
-      <c r="E73" t="inlineStr">
+      <c r="F73" t="inlineStr">
         <is>
           <t>1.00-1.49</t>
         </is>
       </c>
-      <c r="F73" t="n">
+      <c r="G73" t="n">
         <v>6.3</v>
       </c>
-      <c r="G73" t="n">
-        <v>100000</v>
-      </c>
       <c r="H73" t="n">
+        <v>100000</v>
+      </c>
+      <c r="I73" t="n">
         <v>3</v>
       </c>
-      <c r="I73" t="n">
+      <c r="J73" t="n">
         <v>1.5</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
+          <t>RO</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
           <t>VG</t>
         </is>
       </c>
-      <c r="B74" t="inlineStr"/>
       <c r="C74" t="inlineStr"/>
-      <c r="D74" t="inlineStr">
+      <c r="D74" t="inlineStr"/>
+      <c r="E74" t="inlineStr">
         <is>
           <t>NONE</t>
         </is>
       </c>
-      <c r="E74" t="inlineStr">
+      <c r="F74" t="inlineStr">
         <is>
           <t>1.00-1.49</t>
         </is>
       </c>
-      <c r="F74" t="n">
+      <c r="G74" t="n">
         <v>6.3</v>
       </c>
-      <c r="G74" t="n">
-        <v>100000</v>
-      </c>
       <c r="H74" t="n">
+        <v>100000</v>
+      </c>
+      <c r="I74" t="n">
         <v>4</v>
       </c>
-      <c r="I74" t="n">
+      <c r="J74" t="n">
         <v>1.5</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
+          <t>RO</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
           <t>VG</t>
         </is>
       </c>
-      <c r="B75" t="inlineStr"/>
       <c r="C75" t="inlineStr"/>
-      <c r="D75" t="inlineStr">
+      <c r="D75" t="inlineStr"/>
+      <c r="E75" t="inlineStr">
         <is>
           <t>FAINT</t>
         </is>
       </c>
-      <c r="E75" t="inlineStr">
+      <c r="F75" t="inlineStr">
         <is>
           <t>1.00-1.49</t>
         </is>
       </c>
-      <c r="F75" t="n">
+      <c r="G75" t="n">
         <v>6.3</v>
       </c>
-      <c r="G75" t="n">
-        <v>100000</v>
-      </c>
       <c r="H75" t="n">
+        <v>100000</v>
+      </c>
+      <c r="I75" t="n">
         <v>4</v>
       </c>
-      <c r="I75" t="n">
+      <c r="J75" t="n">
         <v>1.5</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
+          <t>RO</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
           <t>VG</t>
         </is>
       </c>
-      <c r="B76" t="inlineStr"/>
       <c r="C76" t="inlineStr"/>
-      <c r="D76" t="inlineStr">
+      <c r="D76" t="inlineStr"/>
+      <c r="E76" t="inlineStr">
         <is>
           <t>NONE</t>
         </is>
       </c>
-      <c r="E76" t="inlineStr">
+      <c r="F76" t="inlineStr">
         <is>
           <t>1.00-1.49</t>
         </is>
       </c>
-      <c r="F76" t="n">
+      <c r="G76" t="n">
         <v>6.3</v>
       </c>
-      <c r="G76" t="n">
-        <v>100000</v>
-      </c>
       <c r="H76" t="n">
+        <v>100000</v>
+      </c>
+      <c r="I76" t="n">
         <v>5</v>
       </c>
-      <c r="I76" t="n">
+      <c r="J76" t="n">
         <v>1.5</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
+          <t>RO</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
           <t>VG</t>
         </is>
       </c>
-      <c r="B77" t="inlineStr"/>
       <c r="C77" t="inlineStr"/>
-      <c r="D77" t="inlineStr">
+      <c r="D77" t="inlineStr"/>
+      <c r="E77" t="inlineStr">
         <is>
           <t>FAINT</t>
         </is>
       </c>
-      <c r="E77" t="inlineStr">
+      <c r="F77" t="inlineStr">
         <is>
           <t>1.00-1.49</t>
         </is>
       </c>
-      <c r="F77" t="n">
+      <c r="G77" t="n">
         <v>6.3</v>
       </c>
-      <c r="G77" t="n">
-        <v>100000</v>
-      </c>
       <c r="H77" t="n">
+        <v>100000</v>
+      </c>
+      <c r="I77" t="n">
         <v>5</v>
       </c>
-      <c r="I77" t="n">
+      <c r="J77" t="n">
         <v>1.5</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
+          <t>RO</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
           <t>VG</t>
         </is>
       </c>
-      <c r="B78" t="inlineStr"/>
       <c r="C78" t="inlineStr"/>
-      <c r="D78" t="inlineStr">
+      <c r="D78" t="inlineStr"/>
+      <c r="E78" t="inlineStr">
         <is>
           <t>NONE</t>
         </is>
       </c>
-      <c r="E78" t="inlineStr">
+      <c r="F78" t="inlineStr">
         <is>
           <t>1.00-1.49</t>
         </is>
       </c>
-      <c r="F78" t="n">
+      <c r="G78" t="n">
         <v>6.3</v>
       </c>
-      <c r="G78" t="n">
-        <v>100000</v>
-      </c>
       <c r="H78" t="n">
+        <v>100000</v>
+      </c>
+      <c r="I78" t="n">
         <v>6</v>
       </c>
-      <c r="I78" t="n">
+      <c r="J78" t="n">
         <v>1.5</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
+          <t>RO</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
           <t>VG</t>
         </is>
       </c>
-      <c r="B79" t="inlineStr"/>
       <c r="C79" t="inlineStr"/>
-      <c r="D79" t="inlineStr">
+      <c r="D79" t="inlineStr"/>
+      <c r="E79" t="inlineStr">
         <is>
           <t>FAINT</t>
         </is>
       </c>
-      <c r="E79" t="inlineStr">
+      <c r="F79" t="inlineStr">
         <is>
           <t>1.00-1.49</t>
         </is>
       </c>
-      <c r="F79" t="n">
+      <c r="G79" t="n">
         <v>6.3</v>
       </c>
-      <c r="G79" t="n">
-        <v>100000</v>
-      </c>
       <c r="H79" t="n">
+        <v>100000</v>
+      </c>
+      <c r="I79" t="n">
         <v>6</v>
       </c>
-      <c r="I79" t="n">
+      <c r="J79" t="n">
         <v>1.5</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
+          <t>RO</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
           <t>VG</t>
         </is>
       </c>
-      <c r="B80" t="inlineStr"/>
       <c r="C80" t="inlineStr"/>
-      <c r="D80" t="inlineStr">
+      <c r="D80" t="inlineStr"/>
+      <c r="E80" t="inlineStr">
         <is>
           <t>NONE</t>
         </is>
       </c>
-      <c r="E80" t="inlineStr">
+      <c r="F80" t="inlineStr">
         <is>
           <t>1.00-1.49</t>
         </is>
       </c>
-      <c r="F80" t="n">
+      <c r="G80" t="n">
         <v>6.3</v>
       </c>
-      <c r="G80" t="n">
-        <v>100000</v>
-      </c>
       <c r="H80" t="n">
+        <v>100000</v>
+      </c>
+      <c r="I80" t="n">
         <v>7</v>
       </c>
-      <c r="I80" t="n">
+      <c r="J80" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
+          <t>RO</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
           <t>VG</t>
         </is>
       </c>
-      <c r="B81" t="inlineStr"/>
       <c r="C81" t="inlineStr"/>
-      <c r="D81" t="inlineStr">
+      <c r="D81" t="inlineStr"/>
+      <c r="E81" t="inlineStr">
         <is>
           <t>FAINT</t>
         </is>
       </c>
-      <c r="E81" t="inlineStr">
+      <c r="F81" t="inlineStr">
         <is>
           <t>1.00-1.49</t>
         </is>
       </c>
-      <c r="F81" t="n">
+      <c r="G81" t="n">
         <v>6.3</v>
       </c>
-      <c r="G81" t="n">
-        <v>100000</v>
-      </c>
       <c r="H81" t="n">
+        <v>100000</v>
+      </c>
+      <c r="I81" t="n">
         <v>7</v>
       </c>
-      <c r="I81" t="n">
+      <c r="J81" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
+          <t>RO</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
           <t>VG</t>
         </is>
       </c>
-      <c r="B82" t="inlineStr"/>
       <c r="C82" t="inlineStr"/>
-      <c r="D82" t="inlineStr">
+      <c r="D82" t="inlineStr"/>
+      <c r="E82" t="inlineStr">
         <is>
           <t>NONE</t>
         </is>
       </c>
-      <c r="E82" t="inlineStr">
+      <c r="F82" t="inlineStr">
         <is>
           <t>1.00-1.49</t>
         </is>
       </c>
-      <c r="F82" t="n">
+      <c r="G82" t="n">
         <v>6.3</v>
       </c>
-      <c r="G82" t="n">
-        <v>100000</v>
-      </c>
       <c r="H82" t="n">
+        <v>100000</v>
+      </c>
+      <c r="I82" t="n">
         <v>8</v>
       </c>
-      <c r="I82" t="n">
+      <c r="J82" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
+          <t>RO</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
           <t>VG</t>
         </is>
       </c>
-      <c r="B83" t="inlineStr"/>
       <c r="C83" t="inlineStr"/>
-      <c r="D83" t="inlineStr">
+      <c r="D83" t="inlineStr"/>
+      <c r="E83" t="inlineStr">
         <is>
           <t>FAINT</t>
         </is>
       </c>
-      <c r="E83" t="inlineStr">
+      <c r="F83" t="inlineStr">
         <is>
           <t>1.00-1.49</t>
         </is>
       </c>
-      <c r="F83" t="n">
+      <c r="G83" t="n">
         <v>6.3</v>
       </c>
-      <c r="G83" t="n">
-        <v>100000</v>
-      </c>
       <c r="H83" t="n">
+        <v>100000</v>
+      </c>
+      <c r="I83" t="n">
         <v>8</v>
       </c>
-      <c r="I83" t="n">
+      <c r="J83" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
+          <t>RO</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
           <t>VG</t>
         </is>
       </c>
-      <c r="B84" t="inlineStr"/>
       <c r="C84" t="inlineStr"/>
-      <c r="D84" t="inlineStr">
+      <c r="D84" t="inlineStr"/>
+      <c r="E84" t="inlineStr">
         <is>
           <t>NONE</t>
         </is>
       </c>
-      <c r="E84" t="inlineStr">
+      <c r="F84" t="inlineStr">
         <is>
           <t>1.00-1.49</t>
         </is>
       </c>
-      <c r="F84" t="n">
+      <c r="G84" t="n">
         <v>6.3</v>
       </c>
-      <c r="G84" t="n">
-        <v>100000</v>
-      </c>
       <c r="H84" t="n">
+        <v>100000</v>
+      </c>
+      <c r="I84" t="n">
         <v>9</v>
       </c>
-      <c r="I84" t="n">
+      <c r="J84" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
+          <t>RO</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
           <t>VG</t>
         </is>
       </c>
-      <c r="B85" t="inlineStr"/>
       <c r="C85" t="inlineStr"/>
-      <c r="D85" t="inlineStr">
+      <c r="D85" t="inlineStr"/>
+      <c r="E85" t="inlineStr">
         <is>
           <t>FAINT</t>
         </is>
       </c>
-      <c r="E85" t="inlineStr">
+      <c r="F85" t="inlineStr">
         <is>
           <t>1.00-1.49</t>
         </is>
       </c>
-      <c r="F85" t="n">
+      <c r="G85" t="n">
         <v>6.3</v>
       </c>
-      <c r="G85" t="n">
-        <v>100000</v>
-      </c>
       <c r="H85" t="n">
+        <v>100000</v>
+      </c>
+      <c r="I85" t="n">
         <v>9</v>
       </c>
-      <c r="I85" t="n">
+      <c r="J85" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
UI for price module upload completed
</commit_message>
<xml_diff>
--- a/miscellenious_discounts/output_files/output_extra_discounts.xlsx
+++ b/miscellenious_discounts/output_files/output_extra_discounts.xlsx
@@ -477,36 +477,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr filterMode="0">
+  <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr fitToPage="0"/>
+    <pageSetUpPr/>
   </sheetPr>
   <dimension ref="A1:C81"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.5625" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" ht="15" customHeight="1" s="3">
-      <c r="A1" s="4" t="inlineStr">
+    <row r="1">
+      <c r="A1" s="6" t="inlineStr">
         <is>
           <t>COLOR</t>
         </is>
       </c>
-      <c r="B1" s="4" t="inlineStr">
+      <c r="B1" s="6" t="inlineStr">
         <is>
           <t>CLARITY</t>
         </is>
       </c>
-      <c r="C1" s="4" t="inlineStr">
+      <c r="C1" s="6" t="inlineStr">
         <is>
           <t>KEY</t>
         </is>
       </c>
     </row>
-    <row r="2" ht="15" customHeight="1" s="3">
+    <row r="2">
       <c r="A2" s="5" t="inlineStr">
         <is>
           <t>D</t>
@@ -521,7 +521,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" ht="15" customHeight="1" s="3">
+    <row r="3">
       <c r="A3" s="5" t="inlineStr">
         <is>
           <t>D</t>
@@ -536,7 +536,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" ht="15" customHeight="1" s="3">
+    <row r="4">
       <c r="A4" s="5" t="inlineStr">
         <is>
           <t>D</t>
@@ -551,7 +551,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" ht="15" customHeight="1" s="3">
+    <row r="5">
       <c r="A5" s="5" t="inlineStr">
         <is>
           <t>D</t>
@@ -566,7 +566,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" ht="15" customHeight="1" s="3">
+    <row r="6">
       <c r="A6" s="5" t="inlineStr">
         <is>
           <t>D</t>
@@ -581,7 +581,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" ht="15" customHeight="1" s="3">
+    <row r="7">
       <c r="A7" s="5" t="inlineStr">
         <is>
           <t>D</t>
@@ -596,7 +596,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" ht="15" customHeight="1" s="3">
+    <row r="8">
       <c r="A8" s="5" t="inlineStr">
         <is>
           <t>D</t>
@@ -611,7 +611,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" ht="15" customHeight="1" s="3">
+    <row r="9">
       <c r="A9" s="5" t="inlineStr">
         <is>
           <t>D</t>
@@ -626,7 +626,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" ht="15" customHeight="1" s="3">
+    <row r="10">
       <c r="A10" s="5" t="inlineStr">
         <is>
           <t>E</t>
@@ -641,7 +641,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" ht="15" customHeight="1" s="3">
+    <row r="11">
       <c r="A11" s="5" t="inlineStr">
         <is>
           <t>E</t>
@@ -656,7 +656,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" ht="15" customHeight="1" s="3">
+    <row r="12">
       <c r="A12" s="5" t="inlineStr">
         <is>
           <t>E</t>
@@ -671,7 +671,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" ht="15" customHeight="1" s="3">
+    <row r="13">
       <c r="A13" s="5" t="inlineStr">
         <is>
           <t>E</t>
@@ -686,7 +686,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" ht="15" customHeight="1" s="3">
+    <row r="14">
       <c r="A14" s="5" t="inlineStr">
         <is>
           <t>E</t>
@@ -701,7 +701,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" ht="15" customHeight="1" s="3">
+    <row r="15">
       <c r="A15" s="5" t="inlineStr">
         <is>
           <t>E</t>
@@ -716,7 +716,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" ht="15" customHeight="1" s="3">
+    <row r="16">
       <c r="A16" s="5" t="inlineStr">
         <is>
           <t>E</t>
@@ -731,7 +731,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" ht="15" customHeight="1" s="3">
+    <row r="17">
       <c r="A17" s="5" t="inlineStr">
         <is>
           <t>E</t>
@@ -746,7 +746,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" ht="15" customHeight="1" s="3">
+    <row r="18">
       <c r="A18" s="5" t="inlineStr">
         <is>
           <t>F</t>
@@ -761,7 +761,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" ht="15" customHeight="1" s="3">
+    <row r="19">
       <c r="A19" s="5" t="inlineStr">
         <is>
           <t>F</t>
@@ -776,7 +776,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" ht="15" customHeight="1" s="3">
+    <row r="20">
       <c r="A20" s="5" t="inlineStr">
         <is>
           <t>F</t>
@@ -791,7 +791,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" ht="15" customHeight="1" s="3">
+    <row r="21">
       <c r="A21" s="5" t="inlineStr">
         <is>
           <t>F</t>
@@ -806,7 +806,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" ht="15" customHeight="1" s="3">
+    <row r="22">
       <c r="A22" s="5" t="inlineStr">
         <is>
           <t>F</t>
@@ -821,7 +821,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" ht="15" customHeight="1" s="3">
+    <row r="23">
       <c r="A23" s="5" t="inlineStr">
         <is>
           <t>F</t>
@@ -836,7 +836,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" ht="15" customHeight="1" s="3">
+    <row r="24">
       <c r="A24" s="5" t="inlineStr">
         <is>
           <t>F</t>
@@ -851,7 +851,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" ht="15" customHeight="1" s="3">
+    <row r="25">
       <c r="A25" s="5" t="inlineStr">
         <is>
           <t>F</t>
@@ -866,7 +866,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" ht="15" customHeight="1" s="3">
+    <row r="26">
       <c r="A26" s="5" t="inlineStr">
         <is>
           <t>G</t>
@@ -881,7 +881,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" ht="15" customHeight="1" s="3">
+    <row r="27">
       <c r="A27" s="5" t="inlineStr">
         <is>
           <t>G</t>
@@ -896,7 +896,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" ht="15" customHeight="1" s="3">
+    <row r="28">
       <c r="A28" s="5" t="inlineStr">
         <is>
           <t>G</t>
@@ -911,7 +911,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" ht="15" customHeight="1" s="3">
+    <row r="29">
       <c r="A29" s="5" t="inlineStr">
         <is>
           <t>G</t>
@@ -926,7 +926,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" ht="15" customHeight="1" s="3">
+    <row r="30">
       <c r="A30" s="5" t="inlineStr">
         <is>
           <t>G</t>
@@ -941,7 +941,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" ht="15" customHeight="1" s="3">
+    <row r="31">
       <c r="A31" s="5" t="inlineStr">
         <is>
           <t>G</t>
@@ -956,7 +956,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" ht="15" customHeight="1" s="3">
+    <row r="32">
       <c r="A32" s="5" t="inlineStr">
         <is>
           <t>G</t>
@@ -971,7 +971,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="33" ht="15" customHeight="1" s="3">
+    <row r="33">
       <c r="A33" s="5" t="inlineStr">
         <is>
           <t>G</t>
@@ -986,7 +986,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="34" ht="15" customHeight="1" s="3">
+    <row r="34">
       <c r="A34" s="5" t="inlineStr">
         <is>
           <t>H</t>
@@ -1001,7 +1001,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" ht="15" customHeight="1" s="3">
+    <row r="35">
       <c r="A35" s="5" t="inlineStr">
         <is>
           <t>H</t>
@@ -1016,7 +1016,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" ht="15" customHeight="1" s="3">
+    <row r="36">
       <c r="A36" s="5" t="inlineStr">
         <is>
           <t>H</t>
@@ -1031,7 +1031,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" ht="15" customHeight="1" s="3">
+    <row r="37">
       <c r="A37" s="5" t="inlineStr">
         <is>
           <t>H</t>
@@ -1046,7 +1046,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" ht="15" customHeight="1" s="3">
+    <row r="38">
       <c r="A38" s="5" t="inlineStr">
         <is>
           <t>H</t>
@@ -1061,7 +1061,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="39" ht="15" customHeight="1" s="3">
+    <row r="39">
       <c r="A39" s="5" t="inlineStr">
         <is>
           <t>H</t>
@@ -1076,7 +1076,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="40" ht="15" customHeight="1" s="3">
+    <row r="40">
       <c r="A40" s="5" t="inlineStr">
         <is>
           <t>H</t>
@@ -1091,7 +1091,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="41" ht="15" customHeight="1" s="3">
+    <row r="41">
       <c r="A41" s="5" t="inlineStr">
         <is>
           <t>H</t>
@@ -1106,7 +1106,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="42" ht="15" customHeight="1" s="3">
+    <row r="42">
       <c r="A42" s="5" t="inlineStr">
         <is>
           <t>I</t>
@@ -1121,7 +1121,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" ht="15" customHeight="1" s="3">
+    <row r="43">
       <c r="A43" s="5" t="inlineStr">
         <is>
           <t>I</t>
@@ -1136,7 +1136,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" ht="15" customHeight="1" s="3">
+    <row r="44">
       <c r="A44" s="5" t="inlineStr">
         <is>
           <t>I</t>
@@ -1151,7 +1151,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" ht="15" customHeight="1" s="3">
+    <row r="45">
       <c r="A45" s="5" t="inlineStr">
         <is>
           <t>I</t>
@@ -1166,7 +1166,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="46" ht="15" customHeight="1" s="3">
+    <row r="46">
       <c r="A46" s="5" t="inlineStr">
         <is>
           <t>I</t>
@@ -1181,7 +1181,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="47" ht="15" customHeight="1" s="3">
+    <row r="47">
       <c r="A47" s="5" t="inlineStr">
         <is>
           <t>I</t>
@@ -1196,7 +1196,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="48" ht="15" customHeight="1" s="3">
+    <row r="48">
       <c r="A48" s="5" t="inlineStr">
         <is>
           <t>I</t>
@@ -1211,7 +1211,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="49" ht="15" customHeight="1" s="3">
+    <row r="49">
       <c r="A49" s="5" t="inlineStr">
         <is>
           <t>I</t>
@@ -1226,7 +1226,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="50" ht="15" customHeight="1" s="3">
+    <row r="50">
       <c r="A50" s="5" t="inlineStr">
         <is>
           <t>J</t>
@@ -1241,7 +1241,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="51" ht="15" customHeight="1" s="3">
+    <row r="51">
       <c r="A51" s="5" t="inlineStr">
         <is>
           <t>J</t>
@@ -1256,7 +1256,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="52" ht="15" customHeight="1" s="3">
+    <row r="52">
       <c r="A52" s="5" t="inlineStr">
         <is>
           <t>J</t>
@@ -1271,7 +1271,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="53" ht="15" customHeight="1" s="3">
+    <row r="53">
       <c r="A53" s="5" t="inlineStr">
         <is>
           <t>J</t>
@@ -1286,7 +1286,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="54" ht="15" customHeight="1" s="3">
+    <row r="54">
       <c r="A54" s="5" t="inlineStr">
         <is>
           <t>J</t>
@@ -1301,7 +1301,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="55" ht="15" customHeight="1" s="3">
+    <row r="55">
       <c r="A55" s="5" t="inlineStr">
         <is>
           <t>J</t>
@@ -1316,7 +1316,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="56" ht="15" customHeight="1" s="3">
+    <row r="56">
       <c r="A56" s="5" t="inlineStr">
         <is>
           <t>J</t>
@@ -1331,7 +1331,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="57" ht="15" customHeight="1" s="3">
+    <row r="57">
       <c r="A57" s="5" t="inlineStr">
         <is>
           <t>J</t>
@@ -1346,7 +1346,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="58" ht="15" customHeight="1" s="3">
+    <row r="58">
       <c r="A58" s="5" t="inlineStr">
         <is>
           <t>K</t>
@@ -1361,7 +1361,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="59" ht="15" customHeight="1" s="3">
+    <row r="59">
       <c r="A59" s="5" t="inlineStr">
         <is>
           <t>K</t>
@@ -1376,7 +1376,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="60" ht="15" customHeight="1" s="3">
+    <row r="60">
       <c r="A60" s="5" t="inlineStr">
         <is>
           <t>K</t>
@@ -1391,7 +1391,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="61" ht="15" customHeight="1" s="3">
+    <row r="61">
       <c r="A61" s="5" t="inlineStr">
         <is>
           <t>K</t>
@@ -1406,7 +1406,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="62" ht="15" customHeight="1" s="3">
+    <row r="62">
       <c r="A62" s="5" t="inlineStr">
         <is>
           <t>K</t>
@@ -1421,7 +1421,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="63" ht="15" customHeight="1" s="3">
+    <row r="63">
       <c r="A63" s="5" t="inlineStr">
         <is>
           <t>K</t>
@@ -1436,7 +1436,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="64" ht="15" customHeight="1" s="3">
+    <row r="64">
       <c r="A64" s="5" t="inlineStr">
         <is>
           <t>K</t>
@@ -1451,7 +1451,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="65" ht="15" customHeight="1" s="3">
+    <row r="65">
       <c r="A65" s="5" t="inlineStr">
         <is>
           <t>K</t>
@@ -1466,7 +1466,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="66" ht="15" customHeight="1" s="3">
+    <row r="66">
       <c r="A66" s="5" t="inlineStr">
         <is>
           <t>L</t>
@@ -1481,7 +1481,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="67" ht="15" customHeight="1" s="3">
+    <row r="67">
       <c r="A67" s="5" t="inlineStr">
         <is>
           <t>L</t>
@@ -1496,7 +1496,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="68" ht="15" customHeight="1" s="3">
+    <row r="68">
       <c r="A68" s="5" t="inlineStr">
         <is>
           <t>L</t>
@@ -1511,7 +1511,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="69" ht="15" customHeight="1" s="3">
+    <row r="69">
       <c r="A69" s="5" t="inlineStr">
         <is>
           <t>L</t>
@@ -1526,7 +1526,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="70" ht="15" customHeight="1" s="3">
+    <row r="70">
       <c r="A70" s="5" t="inlineStr">
         <is>
           <t>L</t>
@@ -1541,7 +1541,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="71" ht="15" customHeight="1" s="3">
+    <row r="71">
       <c r="A71" s="5" t="inlineStr">
         <is>
           <t>L</t>
@@ -1556,7 +1556,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="72" ht="15" customHeight="1" s="3">
+    <row r="72">
       <c r="A72" s="5" t="inlineStr">
         <is>
           <t>L</t>
@@ -1571,7 +1571,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="73" ht="15" customHeight="1" s="3">
+    <row r="73">
       <c r="A73" s="5" t="inlineStr">
         <is>
           <t>L</t>
@@ -1586,7 +1586,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="74" ht="15" customHeight="1" s="3">
+    <row r="74">
       <c r="A74" s="5" t="inlineStr">
         <is>
           <t>M</t>
@@ -1601,7 +1601,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="75" ht="15" customHeight="1" s="3">
+    <row r="75">
       <c r="A75" s="5" t="inlineStr">
         <is>
           <t>M</t>
@@ -1616,7 +1616,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="76" ht="15" customHeight="1" s="3">
+    <row r="76">
       <c r="A76" s="5" t="inlineStr">
         <is>
           <t>M</t>
@@ -1631,7 +1631,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="77" ht="15" customHeight="1" s="3">
+    <row r="77">
       <c r="A77" s="5" t="inlineStr">
         <is>
           <t>M</t>
@@ -1646,7 +1646,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="78" ht="15" customHeight="1" s="3">
+    <row r="78">
       <c r="A78" s="5" t="inlineStr">
         <is>
           <t>M</t>
@@ -1661,7 +1661,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="79" ht="15" customHeight="1" s="3">
+    <row r="79">
       <c r="A79" s="5" t="inlineStr">
         <is>
           <t>M</t>
@@ -1676,7 +1676,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="80" ht="15" customHeight="1" s="3">
+    <row r="80">
       <c r="A80" s="5" t="inlineStr">
         <is>
           <t>M</t>
@@ -1691,7 +1691,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="81" ht="15" customHeight="1" s="3">
+    <row r="81">
       <c r="A81" s="5" t="inlineStr">
         <is>
           <t>M</t>
@@ -1707,9 +1707,7 @@
       </c>
     </row>
   </sheetData>
-  <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup orientation="portrait" paperSize="9" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver" blackAndWhite="0" draft="0" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Created main page function
</commit_message>
<xml_diff>
--- a/miscellenious_discounts/output_files/output_extra_discounts.xlsx
+++ b/miscellenious_discounts/output_files/output_extra_discounts.xlsx
@@ -4500,7 +4500,7 @@
         <v>5</v>
       </c>
       <c r="K58" s="5" t="n">
-        <v>-0.05</v>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="59">
@@ -4541,7 +4541,7 @@
         <v>5</v>
       </c>
       <c r="K59" s="5" t="n">
-        <v>-0.05</v>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="60">

</xml_diff>